<commit_message>
added more benchmark statistics
</commit_message>
<xml_diff>
--- a/benchmark_statistics/rusults.xlsx
+++ b/benchmark_statistics/rusults.xlsx
@@ -252,7 +252,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1114,28 +1114,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0.062392</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.350258</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.073801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.019539</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.276853</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.117099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.030851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.564644</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1406,11 +1406,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="81687544"/>
-        <c:axId val="51676171"/>
+        <c:axId val="75873356"/>
+        <c:axId val="58127632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81687544"/>
+        <c:axId val="75873356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,14 +1426,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51676171"/>
+        <c:crossAx val="58127632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51676171"/>
+        <c:axId val="58127632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,7 +1458,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="81687544"/>
+        <c:crossAx val="75873356"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1493,7 +1493,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1507,7 +1507,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$33</c:f>
+              <c:f>Sheet1!$A$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1526,9 +1526,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -1555,42 +1555,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$J$33</c:f>
+              <c:f>Sheet1!$B$48:$K$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>90145783</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60515282</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>155381520</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>76759933</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16715585</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>463683043</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110675818</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19484490</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>34120048.7657541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>363383125.266464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>276083133.294362</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>383818855.942797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>331204997.126949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403327151.425005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>366419193.039494</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>341318186.595663</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111298811</c:v>
+                  <c:v>334761456.603864</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>219607623.96102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,7 +1607,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$34</c:f>
+              <c:f>Sheet1!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1620,9 +1626,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -1649,42 +1655,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$34:$J$34</c:f>
+              <c:f>Sheet1!$B$49:$K$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>98251995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60826837</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>151407745</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>77096491</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16916255</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>465385467</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>111129564</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19560405</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>37307998.7104795</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>365840502.568174</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>497436542.302941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>387396192.189416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>412199493.165038</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>406382399.966468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>648753708.471252</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>361914722.371269</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>111664597</c:v>
+                  <c:v>633604731.129105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>233199643.493761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1695,7 +1707,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$35</c:f>
+              <c:f>Sheet1!$A$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1714,9 +1726,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -1743,42 +1755,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$35:$J$35</c:f>
+              <c:f>Sheet1!$B$50:$K$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>134959449</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>61304800</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>170113072</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>77749640</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17444049</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>469150558</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>113198576</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19747141</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>51475168.1645992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>371285467.704327</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>925478192.273585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>395775188.471308</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>416464904.741441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>411702786.30707</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>661222084.628146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>366801786.908389</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>112616040</c:v>
+                  <c:v>1152577475.74405</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>235607613.469985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1789,7 +1807,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$36</c:f>
+              <c:f>Sheet1!$A$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1808,9 +1826,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -1837,42 +1855,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$36:$J$36</c:f>
+              <c:f>Sheet1!$B$51:$K$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>188581636</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62306934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>212399873</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>78940114</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18472148</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>477723910</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>116847855</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20134562</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>71668727.501581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>376640798.413811</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1417407111.06366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>401966107.391094</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>469300779.959859</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>418792662.860289</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1023975173.51374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>375497696.797896</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>114751525</c:v>
+                  <c:v>1863726835.68563</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>249290636.042403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1883,7 +1907,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$37</c:f>
+              <c:f>Sheet1!$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1902,9 +1926,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -1931,42 +1955,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$J$37</c:f>
+              <c:f>Sheet1!$B$52:$K$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>328375486</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65240774</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>380752372</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>82386813</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21427114</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500818757</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>126491644</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21227839</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>123968373.624175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>394275542.394392</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1331586009.60345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>419307588.951716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>535062528.092693</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439599281.815772</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1339996440.56485</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>390950661.166157</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120519724</c:v>
+                  <c:v>2632182147.7712</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>266559846.698113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1977,7 +2007,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$38</c:f>
+              <c:f>Sheet1!$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1996,9 +2026,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2025,42 +2055,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$38:$J$38</c:f>
+              <c:f>Sheet1!$B$53:$K$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>88439290</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>73331932</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>869524475</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>91498384</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29862992</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>565996348</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>155608004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24018905</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>32821190.2490148</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>440439959.879157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1593595146.59013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464322098.062499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>576372114.568054</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>496342604.885937</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1526152195.44728</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>441873263.793072</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>139176786</c:v>
+                  <c:v>2626423090.71352</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300847670.763075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2071,7 +2107,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$39</c:f>
+              <c:f>Sheet1!$A$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2090,9 +2126,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2119,42 +2155,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$39:$J$39</c:f>
+              <c:f>Sheet1!$B$54:$K$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>96800828</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60176679</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152709493</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68132654</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16085640</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439441872</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>109126499</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19307875</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>39216339.4615092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1745668339.52193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>741898856.371092</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1655714556.50061</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1356979922.38907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3066372702.53297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1747477885.60082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1054614103.12432</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>108863595</c:v>
+                  <c:v>359605045.403345</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>541624273.255814</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2165,7 +2207,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$40</c:f>
+              <c:f>Sheet1!$A$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2184,9 +2226,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2213,42 +2255,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$40:$J$40</c:f>
+              <c:f>Sheet1!$B$55:$K$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>96800828</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60435755</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>151523384</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68265737</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16282414</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439766103</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>109675985</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19408967</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>39015160.9684061</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1654233180.05146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1964162916.10495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1492147256.8306</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1208701210.00668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3075653070.64476</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2946378277.4554</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>872273920.273246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109329770</c:v>
+                  <c:v>690313429.348959</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>570872180.451128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2259,7 +2307,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$41</c:f>
+              <c:f>Sheet1!$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2278,9 +2326,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2307,42 +2355,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$41:$J$41</c:f>
+              <c:f>Sheet1!$B$56:$K$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>96800828</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60200560</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152818448</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68158455</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16089981</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439548449</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>109183576</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19312167</c:v>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>38857420.1783894</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1317241258.58825</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>579217574.55389</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1254619427.16195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1075174139.65921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2231289685.42029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1287329638.9747</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>825447384.168234</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109048192</c:v>
+                  <c:v>264091000.898481</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>459806909.315238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2353,7 +2407,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$42</c:f>
+              <c:f>Sheet1!$A$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2372,9 +2426,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2401,42 +2455,48 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$42:$J$42</c:f>
+              <c:f>Sheet1!$B$57:$K$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>38311334.7151153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965375576.997051</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436766643.445689</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>923994349.670059</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>824228466.144634</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1588270905.49859</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>932760194.365451</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>626641437.878837</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>193618108.04684</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>355755703.422053</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2447,7 +2507,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$43</c:f>
+              <c:f>Sheet1!$A$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2466,9 +2526,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2495,16 +2555,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$43:$J$43</c:f>
+              <c:f>Sheet1!$B$58:$K$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -2530,6 +2593,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2541,7 +2607,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$44</c:f>
+              <c:f>Sheet1!$A$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2560,9 +2626,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2589,16 +2655,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$44:$J$44</c:f>
+              <c:f>Sheet1!$B$59:$K$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -2624,6 +2693,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2635,7 +2707,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$45</c:f>
+              <c:f>Sheet1!$A$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2654,9 +2726,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$32:$J$32</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>BOOT</c:v>
                 </c:pt>
@@ -2683,16 +2755,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$45:$J$45</c:f>
+              <c:f>Sheet1!$B$60:$K$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v/>
                 </c:pt>
@@ -2718,6 +2793,9 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v/>
                 </c:pt>
               </c:numCache>
@@ -2725,11 +2803,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="92160664"/>
-        <c:axId val="33522646"/>
+        <c:axId val="17288668"/>
+        <c:axId val="7372166"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92160664"/>
+        <c:axId val="17288668"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2745,14 +2823,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33522646"/>
+        <c:crossAx val="7372166"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33522646"/>
+        <c:axId val="7372166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,7 +2855,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92160664"/>
+        <c:crossAx val="17288668"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2812,7 +2890,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2826,7 +2904,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$48</c:f>
+              <c:f>Sheet1!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2843,79 +2921,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$48:$K$48</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>34120048.7657541</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>363383125.266464</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>276083133.294362</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>383818855.942797</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>331204997.126949</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>403327151.425005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>366419193.039494</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>341318186.595663</c:v>
+                  <c:v>2.642018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.166533</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.562807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.050469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.149645</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.302047</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.057086</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>334761456.603864</c:v>
+                  <c:v>0.332472</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>219607623.96102</c:v>
+                  <c:v>0.003489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2926,7 +2966,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$49</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2943,79 +2983,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$49:$K$49</c:f>
+              <c:f>Sheet1!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>37307998.7104795</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>365840502.568174</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>497436542.302941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>387396192.189416</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>412199493.165038</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>406382399.966468</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>648753708.471252</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>361914722.371269</c:v>
+                  <c:v>2.633537</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.166266</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.304376</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.199012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.041039</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.145191</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.171297</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.054047</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>633604731.129105</c:v>
+                  <c:v>0.176237</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>233199643.493761</c:v>
+                  <c:v>0.003366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3026,7 +3028,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$50</c:f>
+              <c:f>Sheet1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3043,79 +3045,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$50:$K$50</c:f>
+              <c:f>Sheet1!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>51475168.1645992</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>371285467.704327</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>925478192.273585</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>395775188.471308</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>416464904.741441</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>411702786.30707</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>661222084.628146</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>366801786.908389</c:v>
+                  <c:v>2.621836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.165115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.183811</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.196449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.041886</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.139537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.171196</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.053836</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1152577475.74405</c:v>
+                  <c:v>0.097708</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>235607613.469985</c:v>
+                  <c:v>0.003415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3126,7 +3090,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$51</c:f>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3143,79 +3107,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$51:$K$51</c:f>
+              <c:f>Sheet1!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>71668727.501581</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>376640798.413811</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1417407111.06366</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>401966107.391094</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>469300779.959859</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>418792662.860289</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1023975173.51374</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>375497696.797896</c:v>
+                  <c:v>2.631296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.165428</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.149851</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.196385</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.039361</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.140717</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.114112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.053621</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1863726835.68563</c:v>
+                  <c:v>0.061571</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>249290636.042403</c:v>
+                  <c:v>0.003396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3226,7 +3152,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$52</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3243,79 +3169,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$52:$K$52</c:f>
+              <c:f>Sheet1!$B$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>123968373.624175</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>394275542.394392</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1331586009.60345</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>419307588.951716</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>535062528.092693</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439599281.815772</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1339996440.56485</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>390950661.166157</c:v>
+                  <c:v>2.648865</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16547</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.285939</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.196483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.040046</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.139262</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.094397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.054298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2632182147.7712</c:v>
+                  <c:v>0.045787</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>266559846.698113</c:v>
+                  <c:v>0.003392</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3326,7 +3214,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$53</c:f>
+              <c:f>Sheet1!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3343,79 +3231,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$53:$K$53</c:f>
+              <c:f>Sheet1!$B$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>32821190.2490148</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>440439959.879157</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1593595146.59013</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>464322098.062499</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>576372114.568054</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>496342604.885937</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1526152195.44728</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>441873263.793072</c:v>
+                  <c:v>2.694579</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.166497</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.545637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.197058</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.051812</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.140334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.101961</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.054357</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2626423090.71352</c:v>
+                  <c:v>0.052991</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>300847670.763075</c:v>
+                  <c:v>0.003499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3426,7 +3276,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$54</c:f>
+              <c:f>Sheet1!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3443,79 +3293,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$K$54</c:f>
+              <c:f>Sheet1!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>39216339.4615092</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1745668339.52193</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>741898856.371092</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1655714556.50061</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1356979922.38907</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3066372702.53297</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1747477885.60082</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1054614103.12432</c:v>
+                  <c:v>2.46838</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.034472</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.205836</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04115</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.011854</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.062448</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.018308</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>359605045.403345</c:v>
+                  <c:v>0.302731</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>541624273.255814</c:v>
+                  <c:v>0.001376</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3526,7 +3338,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$55</c:f>
+              <c:f>Sheet1!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3543,79 +3355,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$55:$K$55</c:f>
+              <c:f>Sheet1!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>39015160.9684061</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1654233180.05146</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1964162916.10495</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1492147256.8306</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1208701210.00668</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3075653070.64476</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2946378277.4554</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>872273920.273246</c:v>
+                  <c:v>2.481108</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.036534</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.077144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.013471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.142983</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.037224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.022251</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>690313429.348959</c:v>
+                  <c:v>0.158377</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>570872180.451128</c:v>
+                  <c:v>0.00133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3626,7 +3400,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$56</c:f>
+              <c:f>Sheet1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3643,79 +3417,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$56:$K$56</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>38857420.1783894</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1317241258.58825</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>579217574.55389</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1254619427.16195</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1075174139.65921</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2231289685.42029</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1287329638.9747</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>825447384.168234</c:v>
+                  <c:v>2.49118</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.045702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.263836</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.054326</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.014965</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.196993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.084814</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.023396</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>264091000.898481</c:v>
+                  <c:v>0.412919</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>459806909.315238</c:v>
+                  <c:v>0.001621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3726,7 +3462,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$57</c:f>
+              <c:f>Sheet1!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3743,79 +3479,41 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$57:$K$57</c:f>
+              <c:f>Sheet1!$B$11:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>2.526689</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.062392</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.350258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.073801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.019539</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.276853</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.117099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.030851</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>0.564644</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>0.002104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3826,7 +3524,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$58</c:f>
+              <c:f>Sheet1!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3843,47 +3541,9 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$58:$K$58</c:f>
+              <c:f>Sheet1!$B$12:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3926,7 +3586,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$59</c:f>
+              <c:f>Sheet1!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3943,47 +3603,9 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$59:$K$59</c:f>
+              <c:f>Sheet1!$B$13:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4026,7 +3648,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$60</c:f>
+              <c:f>Sheet1!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4043,47 +3665,9 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$60:$K$60</c:f>
+              <c:f>Sheet1!$B$14:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4122,11 +3706,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="39469569"/>
-        <c:axId val="80803426"/>
+        <c:axId val="48749504"/>
+        <c:axId val="71652456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39469569"/>
+        <c:axId val="48749504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4142,14 +3726,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80803426"/>
+        <c:crossAx val="71652456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80803426"/>
+        <c:axId val="71652456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4174,7 +3758,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39469569"/>
+        <c:crossAx val="48749504"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4209,7 +3793,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4223,7 +3807,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4240,41 +3824,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$K$2</c:f>
+              <c:f>Sheet1!$B$33:$K$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.642018</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.166533</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.562807</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.19999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.050469</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.149645</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.302047</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.057086</c:v>
+                  <c:v>90145783</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60515282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>155381520</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76759933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16715585</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>463683043</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>110675818</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19484490</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.332472</c:v>
+                  <c:v>111298811</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003489</c:v>
+                  <c:v>766211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4285,7 +3907,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4302,41 +3924,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$K$3</c:f>
+              <c:f>Sheet1!$B$34:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.633537</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.166266</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.304376</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.199012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.041039</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.145191</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.171297</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.054047</c:v>
+                  <c:v>98251995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60826837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>151407745</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77096491</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16916255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>465385467</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111129564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19560405</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.176237</c:v>
+                  <c:v>111664597</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003366</c:v>
+                  <c:v>784950</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4347,7 +4007,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4364,41 +4024,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$K$4</c:f>
+              <c:f>Sheet1!$B$35:$K$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.621836</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.165115</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.183811</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.196449</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.041886</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.139537</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.171196</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.053836</c:v>
+                  <c:v>134959449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61304800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170113072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77749640</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17444049</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>469150558</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113198576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19747141</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.097708</c:v>
+                  <c:v>112616040</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003415</c:v>
+                  <c:v>804600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4409,7 +4107,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4426,41 +4124,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$K$5</c:f>
+              <c:f>Sheet1!$B$36:$K$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.631296</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.165428</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.149851</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.196385</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.039361</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.140717</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.114112</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.053621</c:v>
+                  <c:v>188581636</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62306934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>212399873</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78940114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18472148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>477723910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116847855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20134562</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.061571</c:v>
+                  <c:v>114751525</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003396</c:v>
+                  <c:v>846591</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4471,7 +4207,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>Sheet1!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4488,41 +4224,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$K$6</c:f>
+              <c:f>Sheet1!$B$37:$K$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.648865</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16547</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.285939</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.196483</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.040046</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.139262</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.094397</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.054298</c:v>
+                  <c:v>328375486</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65240774</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>380752372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82386813</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21427114</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500818757</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>126491644</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21227839</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.045787</c:v>
+                  <c:v>120519724</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003392</c:v>
+                  <c:v>904171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4533,7 +4307,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet1!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4550,41 +4324,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$K$7</c:f>
+              <c:f>Sheet1!$B$38:$K$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.694579</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.166497</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.545637</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.197058</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.051812</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.140334</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.101961</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.054357</c:v>
+                  <c:v>88439290</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73331932</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>869524475</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91498384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29862992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>565996348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>155608004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24018905</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.052991</c:v>
+                  <c:v>139176786</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003499</c:v>
+                  <c:v>1052666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4595,7 +4407,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet1!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4612,41 +4424,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$K$8</c:f>
+              <c:f>Sheet1!$B$39:$K$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.46838</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.034472</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.205836</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.04115</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.011854</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.14331</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.062448</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.018308</c:v>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60176679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152709493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68132654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16085640</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439441872</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109126499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19307875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.302731</c:v>
+                  <c:v>108863595</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.001376</c:v>
+                  <c:v>745275</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4657,7 +4507,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4674,41 +4524,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$K$9</c:f>
+              <c:f>Sheet1!$B$40:$K$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.481108</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.036534</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.077144</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.04575</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.013471</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.142983</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.037224</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.022251</c:v>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60435755</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>151523384</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68265737</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16282414</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439766103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109675985</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19408967</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.158377</c:v>
+                  <c:v>109329770</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00133</c:v>
+                  <c:v>759260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4719,7 +4607,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>Sheet1!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4736,41 +4624,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$K$10</c:f>
+              <c:f>Sheet1!$B$41:$K$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.49118</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.045702</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.263836</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.054326</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.014965</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.196993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.084814</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.023396</c:v>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60200560</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152818448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68158455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16089981</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439548449</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109183576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19312167</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.412919</c:v>
+                  <c:v>109048192</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.001621</c:v>
+                  <c:v>745347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4781,7 +4707,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4798,41 +4724,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$K$11</c:f>
+              <c:f>Sheet1!$B$42:$K$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60231713</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152981011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68191707</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16104600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439717565</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109225286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19332515</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>109325303</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>748510</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4843,7 +4807,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>Sheet1!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4860,9 +4824,47 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$K$12</c:f>
+              <c:f>Sheet1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4905,7 +4907,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13</c:f>
+              <c:f>Sheet1!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4922,9 +4924,47 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$44:$K$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4967,7 +5007,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>Sheet1!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4984,9 +5024,47 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:f>Sheet1!$B$45:$K$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5025,11 +5103,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="93895990"/>
-        <c:axId val="72093458"/>
+        <c:axId val="16540548"/>
+        <c:axId val="24406095"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93895990"/>
+        <c:axId val="16540548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5045,14 +5123,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72093458"/>
+        <c:crossAx val="24406095"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72093458"/>
+        <c:axId val="24406095"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5077,7 +5155,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93895990"/>
+        <c:crossAx val="16540548"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5116,16 +5194,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>635400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>144720</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>20520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>131040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>260280</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>234000</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5133,7 +5211,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10821960" y="3233160"/>
+        <a:off x="11608560" y="131040"/>
         <a:ext cx="14843880" cy="8380800"/>
       </xdr:xfrm>
       <a:graphic>
@@ -5146,16 +5224,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>723960</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>65880</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>222480</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5163,8 +5241,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13937400" y="12227760"/>
-        <a:ext cx="15768720" cy="11993760"/>
+        <a:off x="65880" y="9960840"/>
+        <a:ext cx="12557160" cy="11343240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5176,16 +5254,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>681840</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>149400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>-360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>25560</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>90000</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>670680</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5193,8 +5271,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="681840" y="12155400"/>
-        <a:ext cx="12557160" cy="11343240"/>
+        <a:off x="28806120" y="-360"/>
+        <a:ext cx="16777440" cy="10024920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5206,16 +5284,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>634320</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>37800</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>343080</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>642600</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>54360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5223,8 +5301,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="26852760" y="776160"/>
-        <a:ext cx="16777440" cy="10024920"/>
+        <a:off x="13251240" y="8813880"/>
+        <a:ext cx="14422320" cy="9609480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5244,8 +5322,8 @@
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L49" activeCellId="0" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5610,6 +5688,36 @@
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <v>2.526689</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.062392</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.350258</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.073801</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.019539</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.276853</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.117099</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.030851</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0.564644</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.002104</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -5980,6 +6088,36 @@
       <c r="A27" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <v>88511420</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>148743133</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>301724144</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>369915851</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>386020451</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>825738016</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>934963302</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>954295817</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>1063621120</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>1064369630</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -6431,6 +6569,45 @@
       <c r="A42" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="B42" s="0" t="n">
+        <v>96800828</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">C27-B27</f>
+        <v>60231713</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">D27-C27</f>
+        <v>152981011</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">E27-D27</f>
+        <v>68191707</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <f aca="false">F27-E27</f>
+        <v>16104600</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <f aca="false">G27-F27</f>
+        <v>439717565</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <f aca="false">H27-G27</f>
+        <v>109225286</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <f aca="false">I27-H27</f>
+        <v>19332515</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <f aca="false">J27-I27</f>
+        <v>109325303</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <f aca="false">K27-J27</f>
+        <v>748510</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -6890,6 +7067,46 @@
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <f aca="false">B42/B11</f>
+        <v>38311334.7151153</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <f aca="false">C42/C11</f>
+        <v>965375576.997051</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <f aca="false">D42/D11</f>
+        <v>436766643.445689</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">E42/E11</f>
+        <v>923994349.670059</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <f aca="false">F42/F11</f>
+        <v>824228466.144634</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <f aca="false">G42/G11</f>
+        <v>1588270905.49859</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <f aca="false">H42/H11</f>
+        <v>932760194.365451</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <f aca="false">I42/I11</f>
+        <v>626641437.878837</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <f aca="false">J42/J11</f>
+        <v>193618108.04684</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <f aca="false">K42/K11</f>
+        <v>355755703.422053</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added final benchmark statistics
</commit_message>
<xml_diff>
--- a/benchmark_statistics/rusults.xlsx
+++ b/benchmark_statistics/rusults.xlsx
@@ -252,7 +252,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1202,28 +1202,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0.085169</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.471994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.100414</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025954</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.386243</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.041256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.781018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,28 +1290,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0.118512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.650373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.139346</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.035128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.547806</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.227037</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.056159</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.094857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,39 +1378,39 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0.165748</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.901321</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.048486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.773445</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31874</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.077512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.535642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="75873356"/>
-        <c:axId val="58127632"/>
+        <c:axId val="17572500"/>
+        <c:axId val="87721693"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75873356"/>
+        <c:axId val="17572500"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,14 +1426,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="58127632"/>
+        <c:crossAx val="87721693"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58127632"/>
+        <c:axId val="87721693"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,7 +1458,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="75873356"/>
+        <c:crossAx val="17572500"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1493,7 +1493,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1507,7 +1507,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$48</c:f>
+              <c:f>Sheet1!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1526,7 +1526,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1564,39 +1564,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$48:$K$48</c:f>
+              <c:f>Sheet1!$B$33:$K$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>34120048.7657541</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>363383125.266464</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>276083133.294362</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>383818855.942797</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>331204997.126949</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>403327151.425005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>366419193.039494</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>341318186.595663</c:v>
+                  <c:v>90145783</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60515282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>155381520</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76759933</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16715585</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>463683043</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>110675818</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19484490</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>334761456.603864</c:v>
+                  <c:v>111298811</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>219607623.96102</c:v>
+                  <c:v>766211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1607,7 +1607,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$49</c:f>
+              <c:f>Sheet1!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1626,7 +1626,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1664,39 +1664,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$49:$K$49</c:f>
+              <c:f>Sheet1!$B$34:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>37307998.7104795</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>365840502.568174</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>497436542.302941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>387396192.189416</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>412199493.165038</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>406382399.966468</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>648753708.471252</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>361914722.371269</c:v>
+                  <c:v>98251995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60826837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>151407745</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77096491</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16916255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>465385467</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111129564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19560405</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>633604731.129105</c:v>
+                  <c:v>111664597</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>233199643.493761</c:v>
+                  <c:v>784950</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1707,7 +1707,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$50</c:f>
+              <c:f>Sheet1!$A$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1726,7 +1726,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1764,39 +1764,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$50:$K$50</c:f>
+              <c:f>Sheet1!$B$35:$K$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>51475168.1645992</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>371285467.704327</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>925478192.273585</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>395775188.471308</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>416464904.741441</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>411702786.30707</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>661222084.628146</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>366801786.908389</c:v>
+                  <c:v>134959449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61304800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170113072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77749640</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17444049</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>469150558</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113198576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19747141</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1152577475.74405</c:v>
+                  <c:v>112616040</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>235607613.469985</c:v>
+                  <c:v>804600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1807,7 +1807,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$51</c:f>
+              <c:f>Sheet1!$A$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1826,7 +1826,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1864,39 +1864,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$51:$K$51</c:f>
+              <c:f>Sheet1!$B$36:$K$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>71668727.501581</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>376640798.413811</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1417407111.06366</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>401966107.391094</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>469300779.959859</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>418792662.860289</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1023975173.51374</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>375497696.797896</c:v>
+                  <c:v>188581636</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62306934</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>212399873</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78940114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18472148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>477723910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116847855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20134562</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1863726835.68563</c:v>
+                  <c:v>114751525</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>249290636.042403</c:v>
+                  <c:v>846591</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1907,7 +1907,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$52</c:f>
+              <c:f>Sheet1!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1926,7 +1926,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1964,39 +1964,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$52:$K$52</c:f>
+              <c:f>Sheet1!$B$37:$K$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>123968373.624175</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>394275542.394392</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1331586009.60345</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>419307588.951716</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>535062528.092693</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439599281.815772</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1339996440.56485</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>390950661.166157</c:v>
+                  <c:v>328375486</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65240774</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>380752372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82386813</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21427114</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500818757</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>126491644</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21227839</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2632182147.7712</c:v>
+                  <c:v>120519724</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>266559846.698113</c:v>
+                  <c:v>904171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2007,7 +2007,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$53</c:f>
+              <c:f>Sheet1!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2026,7 +2026,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2064,39 +2064,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$53:$K$53</c:f>
+              <c:f>Sheet1!$B$38:$K$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>32821190.2490148</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>440439959.879157</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1593595146.59013</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>464322098.062499</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>576372114.568054</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>496342604.885937</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1526152195.44728</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>441873263.793072</c:v>
+                  <c:v>88439290</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73331932</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>869524475</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91498384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29862992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>565996348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>155608004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24018905</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2626423090.71352</c:v>
+                  <c:v>139176786</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>300847670.763075</c:v>
+                  <c:v>1052666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2107,7 +2107,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$54</c:f>
+              <c:f>Sheet1!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2126,7 +2126,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2164,39 +2164,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$54:$K$54</c:f>
+              <c:f>Sheet1!$B$39:$K$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>39216339.4615092</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1745668339.52193</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>741898856.371092</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1655714556.50061</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1356979922.38907</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3066372702.53297</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1747477885.60082</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1054614103.12432</c:v>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60176679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152709493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68132654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16085640</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439441872</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109126499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19307875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>359605045.403345</c:v>
+                  <c:v>108863595</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>541624273.255814</c:v>
+                  <c:v>745275</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2207,7 +2207,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$55</c:f>
+              <c:f>Sheet1!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2226,7 +2226,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2264,39 +2264,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$55:$K$55</c:f>
+              <c:f>Sheet1!$B$40:$K$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>39015160.9684061</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1654233180.05146</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1964162916.10495</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1492147256.8306</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1208701210.00668</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3075653070.64476</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2946378277.4554</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>872273920.273246</c:v>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60435755</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>151523384</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68265737</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16282414</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439766103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109675985</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19408967</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>690313429.348959</c:v>
+                  <c:v>109329770</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>570872180.451128</c:v>
+                  <c:v>759260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2307,7 +2307,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$56</c:f>
+              <c:f>Sheet1!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2326,7 +2326,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2364,39 +2364,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$56:$K$56</c:f>
+              <c:f>Sheet1!$B$41:$K$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>38857420.1783894</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1317241258.58825</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>579217574.55389</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1254619427.16195</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1075174139.65921</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2231289685.42029</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1287329638.9747</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>825447384.168234</c:v>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60200560</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152818448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68158455</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16089981</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439548449</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109183576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19312167</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>264091000.898481</c:v>
+                  <c:v>109048192</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>459806909.315238</c:v>
+                  <c:v>745347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2407,7 +2407,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$57</c:f>
+              <c:f>Sheet1!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2426,7 +2426,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2464,39 +2464,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$57:$K$57</c:f>
+              <c:f>Sheet1!$B$42:$K$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>38311334.7151153</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>965375576.997051</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>436766643.445689</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>923994349.670059</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>824228466.144634</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1588270905.49859</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>932760194.365451</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>626641437.878837</c:v>
+                  <c:v>96800828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60231713</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>152981011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68191707</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16104600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439717565</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109225286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19332515</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>193618108.04684</c:v>
+                  <c:v>109325303</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>355755703.422053</c:v>
+                  <c:v>748510</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2507,7 +2507,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$58</c:f>
+              <c:f>Sheet1!$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2526,7 +2526,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2564,39 +2564,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$58:$K$58</c:f>
+              <c:f>Sheet1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>96800829</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60275183</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153229908</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68239580</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16118564</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439899763</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109295576</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19357428</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>109746504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>754628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2607,7 +2607,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$59</c:f>
+              <c:f>Sheet1!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2626,7 +2626,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2664,39 +2664,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$59:$K$59</c:f>
+              <c:f>Sheet1!$B$44:$K$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>96800830</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60344902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153573713</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68309624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16135053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>440204390</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109439810</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19380770</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>110523224</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>753732</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2707,7 +2707,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$60</c:f>
+              <c:f>Sheet1!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2726,7 +2726,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:f>Sheet1!$B$32:$K$32</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2764,50 +2764,50 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$60:$K$60</c:f>
+              <c:f>Sheet1!$B$45:$K$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>96800831</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60425899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154046287</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68464033</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16168365</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>440637884</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109661447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19429235</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>111253878</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>755966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="17288668"/>
-        <c:axId val="7372166"/>
+        <c:axId val="69309663"/>
+        <c:axId val="50318389"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="17288668"/>
+        <c:axId val="69309663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2823,14 +2823,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="7372166"/>
+        <c:crossAx val="50318389"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7372166"/>
+        <c:axId val="50318389"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2855,7 +2855,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17288668"/>
+        <c:crossAx val="69309663"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2890,7 +2890,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2904,7 +2904,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2921,41 +2921,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$K$2</c:f>
+              <c:f>Sheet1!$B$48:$K$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.642018</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.166533</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.562807</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.19999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.050469</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.149645</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.302047</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.057086</c:v>
+                  <c:v>34120048.7657541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>363383125.266464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>276083133.294362</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>383818855.942797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>331204997.126949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>403327151.425005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>366419193.039494</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>341318186.595663</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.332472</c:v>
+                  <c:v>334761456.603864</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003489</c:v>
+                  <c:v>219607623.96102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2966,7 +3004,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2983,41 +3021,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$K$3</c:f>
+              <c:f>Sheet1!$B$49:$K$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.633537</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.166266</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.304376</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.199012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.041039</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.145191</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.171297</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.054047</c:v>
+                  <c:v>37307998.7104795</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>365840502.568174</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>497436542.302941</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>387396192.189416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>412199493.165038</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>406382399.966468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>648753708.471252</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>361914722.371269</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.176237</c:v>
+                  <c:v>633604731.129105</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003366</c:v>
+                  <c:v>233199643.493761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3028,7 +3104,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3045,41 +3121,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$K$4</c:f>
+              <c:f>Sheet1!$B$50:$K$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.621836</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.165115</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.183811</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.196449</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.041886</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.139537</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.171196</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.053836</c:v>
+                  <c:v>51475168.1645992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>371285467.704327</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>925478192.273585</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>395775188.471308</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>416464904.741441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>411702786.30707</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>661222084.628146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>366801786.908389</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.097708</c:v>
+                  <c:v>1152577475.74405</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003415</c:v>
+                  <c:v>235607613.469985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3090,7 +3204,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3107,41 +3221,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$K$5</c:f>
+              <c:f>Sheet1!$B$51:$K$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.631296</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.165428</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.149851</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.196385</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.039361</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.140717</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.114112</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.053621</c:v>
+                  <c:v>71668727.501581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>376640798.413811</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1417407111.06366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>401966107.391094</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>469300779.959859</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>418792662.860289</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1023975173.51374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>375497696.797896</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.061571</c:v>
+                  <c:v>1863726835.68563</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003396</c:v>
+                  <c:v>249290636.042403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3152,7 +3304,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>Sheet1!$A$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3169,41 +3321,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$K$6</c:f>
+              <c:f>Sheet1!$B$52:$K$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.648865</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16547</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.285939</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.196483</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.040046</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.139262</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.094397</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.054298</c:v>
+                  <c:v>123968373.624175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>394275542.394392</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1331586009.60345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>419307588.951716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>535062528.092693</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>439599281.815772</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1339996440.56485</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>390950661.166157</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.045787</c:v>
+                  <c:v>2632182147.7712</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003392</c:v>
+                  <c:v>266559846.698113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3214,7 +3404,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet1!$A$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3231,41 +3421,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$K$7</c:f>
+              <c:f>Sheet1!$B$53:$K$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.694579</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.166497</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.545637</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.197058</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.051812</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.140334</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.101961</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.054357</c:v>
+                  <c:v>32821190.2490148</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>440439959.879157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1593595146.59013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>464322098.062499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>576372114.568054</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>496342604.885937</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1526152195.44728</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>441873263.793072</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.052991</c:v>
+                  <c:v>2626423090.71352</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.003499</c:v>
+                  <c:v>300847670.763075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3276,7 +3504,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet1!$A$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3293,41 +3521,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$K$8</c:f>
+              <c:f>Sheet1!$B$54:$K$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.46838</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.034472</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.205836</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.04115</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.011854</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.14331</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.062448</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.018308</c:v>
+                  <c:v>39216339.4615092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1745668339.52193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>741898856.371092</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1655714556.50061</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1356979922.38907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3066372702.53297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1747477885.60082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1054614103.12432</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.302731</c:v>
+                  <c:v>359605045.403345</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.001376</c:v>
+                  <c:v>541624273.255814</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3338,7 +3604,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3355,41 +3621,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$K$9</c:f>
+              <c:f>Sheet1!$B$55:$K$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.481108</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.036534</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.077144</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.04575</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.013471</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.142983</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.037224</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.022251</c:v>
+                  <c:v>39015160.9684061</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1654233180.05146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1964162916.10495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1492147256.8306</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1208701210.00668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3075653070.64476</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2946378277.4554</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>872273920.273246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.158377</c:v>
+                  <c:v>690313429.348959</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00133</c:v>
+                  <c:v>570872180.451128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3400,7 +3704,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>Sheet1!$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3417,41 +3721,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$K$10</c:f>
+              <c:f>Sheet1!$B$56:$K$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.49118</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.045702</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.263836</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.054326</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.014965</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.196993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.084814</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.023396</c:v>
+                  <c:v>38857420.1783894</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1317241258.58825</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>579217574.55389</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1254619427.16195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1075174139.65921</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2231289685.42029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1287329638.9747</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>825447384.168234</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.412919</c:v>
+                  <c:v>264091000.898481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.001621</c:v>
+                  <c:v>459806909.315238</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3462,7 +3804,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$A$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3479,41 +3821,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$K$11</c:f>
+              <c:f>Sheet1!$B$57:$K$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.526689</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.062392</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.350258</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.073801</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.019539</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.276853</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.117099</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.030851</c:v>
+                  <c:v>38311334.7151153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>965375576.997051</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>436766643.445689</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>923994349.670059</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>824228466.144634</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1588270905.49859</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>932760194.365451</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>626641437.878837</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.564644</c:v>
+                  <c:v>193618108.04684</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.002104</c:v>
+                  <c:v>355755703.422053</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3524,7 +3904,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>Sheet1!$A$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3541,41 +3921,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$K$12</c:f>
+              <c:f>Sheet1!$B$58:$K$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>37557724.719755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>707712700.630511</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>324643762.420709</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>679582329.157289</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>621043538.568236</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1138919703.39916</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>674372653.791572</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>469202734.14776</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>140517253.123488</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>285843939.393939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3586,7 +4004,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13</c:f>
+              <c:f>Sheet1!$A$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3603,41 +4021,79 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$K$13</c:f>
+              <c:f>Sheet1!$B$59:$K$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>36511971.1467376</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509188115.971378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>236131747.474142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>490215894.248848</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>459321709.177864</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>803577160.527632</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482035130.837705</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>345105325.949536</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>100947634.257259</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>218346465.816918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3648,7 +4104,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>Sheet1!$A$60</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3665,52 +4121,90 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$47:$K$47</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BOOT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>JPEG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCEAN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EPIC</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FFT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>GSM</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>ADPCM</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>RADIX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHUTDOWN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$K$14</c:f>
+              <c:f>Sheet1!$B$60:$K$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
+                  <c:v>35055884.6845124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>364564875.594276</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170911680.744152</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>351223685.425537</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>333464608.340552</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>569708103.355765</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344046705.779005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250660994.426669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>72447795.7753174</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>159789896.427817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="48749504"/>
-        <c:axId val="71652456"/>
+        <c:axId val="66314445"/>
+        <c:axId val="78103271"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48749504"/>
+        <c:axId val="66314445"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,14 +4220,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="71652456"/>
+        <c:crossAx val="78103271"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71652456"/>
+        <c:axId val="78103271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3758,1404 +4252,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="48749504"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_TIMING_1GHZ_P1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$33:$K$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>90145783</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60515282</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>155381520</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>76759933</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16715585</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>463683043</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110675818</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19484490</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>111298811</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>766211</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_TIMING_1GHZ_P2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$34:$K$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>98251995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60826837</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>151407745</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>77096491</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16916255</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>465385467</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>111129564</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19560405</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>111664597</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>784950</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_TIMING_1GHZ_P4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$35:$K$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>134959449</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>61304800</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>170113072</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>77749640</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17444049</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>469150558</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>113198576</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19747141</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>112616040</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>804600</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_TIMING_1GHZ_P8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="579d1c"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$36:$K$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>188581636</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62306934</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>212399873</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>78940114</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18472148</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>477723910</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>116847855</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20134562</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>114751525</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>846591</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_TIMING_1GHZ_P16</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="7e0021"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$37:$K$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>328375486</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65240774</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>380752372</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>82386813</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21427114</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500818757</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>126491644</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21227839</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>120519724</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>904171</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_TIMING_1GHZ_P32</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="83caff"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$38:$K$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>88439290</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>73331932</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>869524475</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>91498384</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29862992</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>565996348</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>155608004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24018905</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>139176786</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1052666</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$39</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_DETAILED_1GHZ_P1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="314004"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$39:$K$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>96800828</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60176679</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152709493</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68132654</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16085640</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439441872</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>109126499</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19307875</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>108863595</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>745275</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$40</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_DETAILED_1GHZ_P2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="aecf00"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$40:$K$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>96800828</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60435755</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>151523384</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68265737</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16282414</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439766103</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>109675985</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19408967</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>109329770</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>759260</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$41</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_DETAILED_710MHZ_P1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4b1f6f"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$41:$K$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>96800828</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60200560</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152818448</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68158455</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16089981</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439548449</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>109183576</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19312167</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>109048192</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>745347</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_DETAILED_500MHZ_P1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff950e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$42:$K$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>96800828</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>60231713</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>152981011</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>68191707</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16104600</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>439717565</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>109225286</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19332515</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>109325303</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>748510</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_DETAILED_354MHZ_P1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c5000b"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$43:$K$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_DETAILED_250MHZ_P1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="0084d1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$44:$K$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="12"/>
-          <c:order val="12"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ALPHA_DETAILED_177MHZ_P1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$32:$K$32</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>BOOT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>JPEG</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>OCEAN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EPIC</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FFT</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>GSM</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>LU</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>ADPCM</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RADIX</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHUTDOWN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$45:$K$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:axId val="16540548"/>
-        <c:axId val="24406095"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="16540548"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="24406095"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="24406095"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="16540548"/>
+        <c:crossAx val="66314445"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5195,15 +4292,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:colOff>24480</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>234000</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>59040</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>367200</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5211,8 +4308,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11608560" y="131040"/>
-        <a:ext cx="14843880" cy="8380800"/>
+        <a:off x="11612520" y="171360"/>
+        <a:ext cx="15785640" cy="8457840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5224,16 +4321,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>37800</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>222480</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>314640</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5241,8 +4338,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="65880" y="9960840"/>
-        <a:ext cx="12557160" cy="11343240"/>
+        <a:off x="11625840" y="8935920"/>
+        <a:ext cx="15719760" cy="7943040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5254,16 +4351,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>149400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>-360</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1360080</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>670680</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>257400</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5271,42 +4368,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28806120" y="-360"/>
-        <a:ext cx="16777440" cy="10024920"/>
+        <a:off x="11546640" y="17632800"/>
+        <a:ext cx="15741720" cy="9473760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>37800</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>642600</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="13251240" y="8813880"/>
-        <a:ext cx="14422320" cy="9609480"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5322,8 +4389,8 @@
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L49" activeCellId="0" sqref="L49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H67" activeCellId="0" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5723,16 +4790,106 @@
       <c r="A12" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B12" s="0" t="n">
+        <v>2.577388</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.085169</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.471994</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.100414</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.025954</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.386243</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.16207</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.041256</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0.781018</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.00264</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="B13" s="0" t="n">
+        <v>2.651208</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.118512</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.650373</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.139346</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.035128</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.547806</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.227037</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.056159</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1.094857</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0.003452</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="B14" s="0" t="n">
+        <v>2.761329</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.165748</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0.901321</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.19493</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.048486</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.773445</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.31874</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.077512</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1.535642</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0.004731</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -6123,16 +5280,106 @@
       <c r="A28" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B28" s="0" t="n">
+        <v>89491324</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>149766507</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>302996415</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>371235995</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>387354559</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>827254322</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>936549898</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>955907326</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>1065653830</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>1066408458</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="B29" s="0" t="n">
+        <v>90191407</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>150536309</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>304110022</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>372419646</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>388554699</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>828759089</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>938198899</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>957579669</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>1068102893</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>1068856625</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="B30" s="0" t="n">
+        <v>90814524</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>151240423</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>305286710</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>373750743</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>389919108</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>830556992</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>940218439</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>959647674</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>1070901552</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>1071657518</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -6613,16 +5860,133 @@
       <c r="A43" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B43" s="0" t="n">
+        <v>96800829</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <f aca="false">C28-B28</f>
+        <v>60275183</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <f aca="false">D28-C28</f>
+        <v>153229908</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">E28-D28</f>
+        <v>68239580</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <f aca="false">F28-E28</f>
+        <v>16118564</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <f aca="false">G28-F28</f>
+        <v>439899763</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <f aca="false">H28-G28</f>
+        <v>109295576</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <f aca="false">I28-H28</f>
+        <v>19357428</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <f aca="false">J28-I28</f>
+        <v>109746504</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <f aca="false">K28-J28</f>
+        <v>754628</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="B44" s="0" t="n">
+        <v>96800830</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <f aca="false">C29-B29</f>
+        <v>60344902</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">D29-C29</f>
+        <v>153573713</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">E29-D29</f>
+        <v>68309624</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">F29-E29</f>
+        <v>16135053</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <f aca="false">G29-F29</f>
+        <v>440204390</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <f aca="false">H29-G29</f>
+        <v>109439810</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <f aca="false">I29-H29</f>
+        <v>19380770</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <f aca="false">J29-I29</f>
+        <v>110523224</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <f aca="false">K29-J29</f>
+        <v>753732</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="B45" s="0" t="n">
+        <v>96800831</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <f aca="false">C30-B30</f>
+        <v>60425899</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">D30-C30</f>
+        <v>154046287</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">E30-D30</f>
+        <v>68464033</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">F30-E30</f>
+        <v>16168365</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <f aca="false">G30-F30</f>
+        <v>440637884</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <f aca="false">H30-G30</f>
+        <v>109661447</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <f aca="false">I30-H30</f>
+        <v>19429235</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <f aca="false">J30-I30</f>
+        <v>111253878</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <f aca="false">K30-J30</f>
+        <v>755966</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -7113,15 +6477,135 @@
       <c r="A58" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B58" s="0" t="n">
+        <f aca="false">B43/B12</f>
+        <v>37557724.719755</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <f aca="false">C43/C12</f>
+        <v>707712700.630511</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <f aca="false">D43/D12</f>
+        <v>324643762.420709</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <f aca="false">E43/E12</f>
+        <v>679582329.157289</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <f aca="false">F43/F12</f>
+        <v>621043538.568236</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <f aca="false">G43/G12</f>
+        <v>1138919703.39916</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <f aca="false">H43/H12</f>
+        <v>674372653.791572</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <f aca="false">I43/I12</f>
+        <v>469202734.14776</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <f aca="false">J43/J12</f>
+        <v>140517253.123488</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <f aca="false">K43/K12</f>
+        <v>285843939.393939</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="B59" s="0" t="n">
+        <f aca="false">B44/B13</f>
+        <v>36511971.1467376</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <f aca="false">C44/C13</f>
+        <v>509188115.971378</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <f aca="false">D44/D13</f>
+        <v>236131747.474142</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <f aca="false">E44/E13</f>
+        <v>490215894.248848</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <f aca="false">F44/F13</f>
+        <v>459321709.177864</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <f aca="false">G44/G13</f>
+        <v>803577160.527632</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <f aca="false">H44/H13</f>
+        <v>482035130.837705</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <f aca="false">I44/I13</f>
+        <v>345105325.949536</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <f aca="false">J44/J13</f>
+        <v>100947634.257259</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <f aca="false">K44/K13</f>
+        <v>218346465.816918</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <f aca="false">B45/B14</f>
+        <v>35055884.6845124</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <f aca="false">C45/C14</f>
+        <v>364564875.594276</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <f aca="false">D45/D14</f>
+        <v>170911680.744152</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <f aca="false">E45/E14</f>
+        <v>351223685.425537</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <f aca="false">F45/F14</f>
+        <v>333464608.340552</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <f aca="false">G45/G14</f>
+        <v>569708103.355765</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <f aca="false">H45/H14</f>
+        <v>344046705.779005</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <f aca="false">I45/I14</f>
+        <v>250660994.426669</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <f aca="false">J45/J14</f>
+        <v>72447795.7753174</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <f aca="false">K45/K14</f>
+        <v>159789896.427817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>